<commit_message>
Deploying to gh-pages from  @ ff1563c2b68c8e95145f392fb87fb8666a6fd4e3 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/16.1.1.xlsx
+++ b/en/downloads/data-excel/16.1.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -62,15 +62,6 @@
   </si>
   <si>
     <t>г. Ош на 100 000 чел.</t>
-  </si>
-  <si>
-    <t>*КР ИИМдин маалыматтары боюнча</t>
-  </si>
-  <si>
-    <t>*по данным МВД КР</t>
-  </si>
-  <si>
-    <t>*according to the MIA of the KR</t>
   </si>
   <si>
     <t>Атайлап өлтүрүлгөндөрдүн саны</t>
@@ -149,9 +140,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -332,10 +320,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -699,16 +687,19 @@
       <c r="I3" s="7">
         <v>2019</v>
       </c>
+      <c r="J3" s="7">
+        <v>2020</v>
+      </c>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="20">
         <v>4.5355634918299268</v>
@@ -728,540 +719,597 @@
       <c r="I4" s="20">
         <v>2.5752932193602573</v>
       </c>
+      <c r="J4" s="20">
+        <v>2.6217442343851403</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="21">
+        <v>28</v>
+      </c>
+      <c r="D5" s="22">
         <v>262</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="22">
         <v>262</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="22">
         <v>209</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="22">
         <v>232</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="22">
         <v>196</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="22">
         <v>168</v>
+      </c>
+      <c r="J5" s="22">
+        <v>174</v>
       </c>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="22">
+        <v>29</v>
+      </c>
+      <c r="D6" s="21">
         <v>1.8723202416541327</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="21">
         <v>1.6240555102173393</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>1.588833676918616</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>1.1682424959890341</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <v>2.2851701975720067</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="21">
         <v>2.0470257646106464</v>
+      </c>
+      <c r="J6" s="21">
+        <v>2.3711940056215539</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="21">
+        <v>28</v>
+      </c>
+      <c r="D7" s="22">
         <v>9</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="22">
         <v>8</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="22">
         <v>6</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="22">
         <v>12</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="22">
         <v>11</v>
+      </c>
+      <c r="J7" s="22">
+        <v>13</v>
       </c>
       <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="22">
+        <v>30</v>
+      </c>
+      <c r="D8" s="21">
         <v>3.5637982248721043</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <v>2.9654955866448032</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="21">
         <v>2.481323760557391</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21">
         <v>1.9318331668877076</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
         <v>1.811544976132895</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="21">
         <v>1.9374369323915239</v>
+      </c>
+      <c r="J8" s="21">
+        <v>2.0624821020182971</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="21">
+        <v>28</v>
+      </c>
+      <c r="D9" s="22">
         <v>40</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="22">
         <v>34</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="22">
         <v>29</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="22">
         <v>23</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="22">
         <v>22</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="22">
         <v>24</v>
+      </c>
+      <c r="J9" s="22">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="22">
+        <v>31</v>
+      </c>
+      <c r="D10" s="21">
         <v>6.2514281279775128</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <v>6.1691102015809944</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="21">
         <v>4.1949828005705179</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="21">
         <v>4.7620723710772426</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="21">
         <v>3.4710524435188308</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <v>4.8382219534321136</v>
+      </c>
+      <c r="J10" s="21">
+        <v>2.1915275544744022</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="21">
+        <v>28</v>
+      </c>
+      <c r="D11" s="22">
         <v>29</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="22">
         <v>29</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="22">
         <v>20</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="22">
         <v>23</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="22">
         <v>17</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="22">
         <v>24</v>
+      </c>
+      <c r="J11" s="22">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="22">
+        <v>32</v>
+      </c>
+      <c r="D12" s="21">
         <v>3.6424034034617403</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <v>2.8812735228971205</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>2.4907220603252882</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="21">
         <v>2.1135765590269093</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="21">
         <v>2.0902427468576685</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="21">
         <v>2.4169518094337081</v>
+      </c>
+      <c r="J12" s="21">
+        <v>3.0807147258163892</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="21">
+        <v>28</v>
+      </c>
+      <c r="D13" s="22">
         <v>10</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="22">
         <v>8</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="22">
         <v>7</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="22">
         <v>6</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="22">
         <v>6</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="22">
         <v>7</v>
+      </c>
+      <c r="J13" s="22">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="22">
+        <v>33</v>
+      </c>
+      <c r="D14" s="21">
         <v>1.3025645868509361</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="21">
         <v>1.8258953238026892</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>1.08735752703831</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="21">
         <v>0.83712194431464837</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="21">
         <v>1.3414186097984668</v>
       </c>
-      <c r="I14" s="22">
-        <v>0.95025488759946608</v>
+      <c r="I14" s="21">
+        <v>1.0964479472301532</v>
+      </c>
+      <c r="J14" s="21">
+        <v>0.79042919586763627</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="21">
+        <v>28</v>
+      </c>
+      <c r="D15" s="22">
         <v>16</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="22">
         <v>23</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="22">
         <v>14</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="22">
         <v>11</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="22">
         <v>18</v>
       </c>
-      <c r="I15" s="21">
-        <v>13</v>
+      <c r="I15" s="22">
+        <v>15</v>
+      </c>
+      <c r="J15" s="22">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="22">
+        <v>34</v>
+      </c>
+      <c r="D16" s="21">
         <v>3.2359056086333959</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="21">
         <v>0</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="21">
         <v>3.5273368606701938</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="21">
         <v>4.2474486348313958</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
         <v>0.7592092076892708</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="21">
         <v>1.8701376421304607</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="21">
+        <v>1.8450593002059086</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="21">
+        <v>38</v>
+      </c>
+      <c r="D17" s="22">
         <v>8</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="22">
         <v>0</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="22">
         <v>9</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="22">
         <v>11</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="22">
         <v>2</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="22">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="22">
+        <v>35</v>
+      </c>
+      <c r="D18" s="21">
         <v>9.9963346772849953</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="21">
         <v>9.803070952824692</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="21">
         <v>8.3961015574768396</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="21">
         <v>8.136890709623664</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="21">
         <v>6.5878042742099145</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="21">
         <v>3.6462739247659091</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="21">
+        <v>5.128289284747237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="21">
+        <v>28</v>
+      </c>
+      <c r="D19" s="22">
         <v>87</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="22">
         <v>87</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="22">
         <v>76</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="22">
         <v>75</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="22">
         <v>62</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="22">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="21">
+        <v>6.9343984569363188</v>
+      </c>
+      <c r="E20" s="21">
+        <v>6.2600356196026752</v>
+      </c>
+      <c r="F20" s="21">
+        <v>4.0800963718763041</v>
+      </c>
+      <c r="G20" s="21">
+        <v>6.0869374322703482</v>
+      </c>
+      <c r="H20" s="21">
+        <v>4.6726924930274665</v>
+      </c>
+      <c r="I20" s="21">
+        <v>3.6056038674845698</v>
+      </c>
+      <c r="J20" s="21">
+        <v>3.537927984544841</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="22">
-        <v>6.9343984569363188</v>
-      </c>
-      <c r="E20" s="22">
-        <v>6.2600356196026752</v>
-      </c>
-      <c r="F20" s="22">
-        <v>4.0800963718763041</v>
-      </c>
-      <c r="G20" s="22">
-        <v>6.0869374322703482</v>
-      </c>
-      <c r="H20" s="22">
-        <v>4.6726924930274665</v>
-      </c>
-      <c r="I20" s="22">
-        <v>3.6056038674845698</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="C21" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="21">
+        <v>28</v>
+      </c>
+      <c r="D21" s="22">
         <v>65</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="22">
         <v>60</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="22">
         <v>40</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="22">
         <v>61</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="22">
         <v>48</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="22">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="22">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="22">
+        <v>37</v>
+      </c>
+      <c r="D22" s="21">
         <v>4.4396430526985631</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <v>4.35172056151701</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="21">
         <v>2.128218043032569</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="21">
         <v>5.5398209252885904</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="21">
         <v>4.0072665099380211</v>
       </c>
-      <c r="I22" s="22">
-        <v>3.5196621124372061</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="21">
+        <v>2.8797235465395321</v>
+      </c>
+      <c r="J22" s="21">
+        <v>3.4144100520231935</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="23">
         <v>12</v>
@@ -1279,19 +1327,16 @@
         <v>12</v>
       </c>
       <c r="I23" s="23">
+        <v>9</v>
+      </c>
+      <c r="J23" s="23">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>18</v>
-      </c>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>

</xml_diff>